<commit_message>
new polarity with google translate (unlimited)
</commit_message>
<xml_diff>
--- a/Data/Result1.xlsx
+++ b/Data/Result1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\ai_chatbot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D10CD6-1A82-4DC2-A765-C0980042A4B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECB8FE3-0F80-43BB-A5AD-1A0BC734FF58}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12470,8 +12470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A667C20-C679-440D-8059-3AB375A4F294}">
   <dimension ref="A1:T176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W106" sqref="W106"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="X81" sqref="X74:Z81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13032,61 +13032,60 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
+      <c r="D10" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="3">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="1">
         <v>0.2</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="1">
         <v>0.8</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="1">
         <v>-0.1</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="1">
         <v>-0.1</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10">
         <v>-0.1</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10" s="1">
         <v>-0.1</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="1">
         <v>-0.1</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10">
         <v>-7.4999999999999997E-2</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10">
         <v>4.7619047619047603E-2</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="Q10">
         <v>21</v>
       </c>
-      <c r="R10" s="3" t="str">
+      <c r="R10" t="str">
         <f t="shared" si="0"/>
         <v>Renuncia/Despido/Desahucio</v>
       </c>
-      <c r="S10" s="3">
+      <c r="S10">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="T10" s="3">
+      <c r="T10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -23111,7 +23110,7 @@
         <v>-1</v>
       </c>
       <c r="O174" s="6">
-        <v>0.26</v>
+        <v>0</v>
       </c>
       <c r="P174" s="6">
         <v>0</v>

</xml_diff>

<commit_message>
0.9 as penalty improves, yandex as translator
</commit_message>
<xml_diff>
--- a/Data/Result1.xlsx
+++ b/Data/Result1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\ai_chatbot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECB8FE3-0F80-43BB-A5AD-1A0BC734FF58}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D971C3D6-49A0-420D-BD97-C76EAC9FA648}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12470,8 +12470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A667C20-C679-440D-8059-3AB375A4F294}">
   <dimension ref="A1:T176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="X81" sqref="X74:Z81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T173" sqref="T173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12549,25 +12549,25 @@
         <v>16</v>
       </c>
       <c r="H2" s="1">
-        <v>-5.7142857142857099E-2</v>
+        <v>-1.6571428571428499</v>
       </c>
       <c r="I2">
         <v>2.8571428571428501</v>
       </c>
       <c r="J2" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="K2" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L2" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M2" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N2" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -12617,19 +12617,19 @@
         <v>1.4391025641025601</v>
       </c>
       <c r="J3">
-        <v>0.17884615384615299</v>
+        <v>-0.62115384615384595</v>
       </c>
       <c r="K3" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L3" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M3" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N3" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -12676,22 +12676,22 @@
         <v>4.0854700854700798</v>
       </c>
       <c r="I4" s="1">
-        <v>-0.146153846153846</v>
+        <v>-2.5461538461538402</v>
       </c>
       <c r="J4" s="1">
-        <v>-9.4871794871794896E-2</v>
+        <v>-2.49487179487179</v>
       </c>
       <c r="K4" s="1">
-        <v>4.4444444444444398E-2</v>
+        <v>-3.1555555555555501</v>
       </c>
       <c r="L4" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="M4" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="N4" s="1">
-        <v>-0.28888888888888797</v>
+        <v>-3.48888888888888</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -12738,22 +12738,22 @@
         <v>1.86733556298773</v>
       </c>
       <c r="I5" s="1">
-        <v>6.3879598662207299E-2</v>
+        <v>-0.736120401337792</v>
       </c>
       <c r="J5">
         <v>0.83835005574136001</v>
       </c>
       <c r="K5" s="1">
-        <v>-0.15652173913043399</v>
+        <v>-1.75652173913043</v>
       </c>
       <c r="L5" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M5" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N5" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -12806,16 +12806,16 @@
         <v>0.10256410256410201</v>
       </c>
       <c r="K6">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L6">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="M6">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N6">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O6">
         <v>0.7</v>
@@ -12868,16 +12868,16 @@
         <v>0.10256410256410201</v>
       </c>
       <c r="K7">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L7">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="M7">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N7">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O7">
         <v>0.7</v>
@@ -12921,25 +12921,25 @@
         <v>27</v>
       </c>
       <c r="H8" s="1">
-        <v>2.16410256410256</v>
+        <v>-1.03589743589743</v>
       </c>
       <c r="I8" s="1">
-        <v>-0.54615384615384599</v>
+        <v>-6.1461538461538403</v>
       </c>
       <c r="J8">
         <v>5.94871794871794</v>
       </c>
       <c r="K8" s="1">
-        <v>-0.89999999999999902</v>
+        <v>-8.1</v>
       </c>
       <c r="L8" s="1">
-        <v>-0.89999999999999902</v>
+        <v>-8.1</v>
       </c>
       <c r="M8" s="1">
-        <v>-0.46666666666666601</v>
+        <v>-6.86666666666666</v>
       </c>
       <c r="N8" s="1">
-        <v>-0.89999999999999902</v>
+        <v>-8.1</v>
       </c>
       <c r="O8">
         <v>0.23749999999999999</v>
@@ -12986,25 +12986,25 @@
         <v>29</v>
       </c>
       <c r="H9" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="I9" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="J9" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="K9" s="1">
-        <v>0.133333333333333</v>
+        <v>-1.4666666666666599</v>
       </c>
       <c r="L9">
         <v>2.3333333333333299</v>
       </c>
       <c r="M9" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N9" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O9">
         <v>0.15</v>
@@ -13054,19 +13054,19 @@
         <v>0.8</v>
       </c>
       <c r="J10" s="1">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="K10" s="1">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L10">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="M10" s="1">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N10" s="1">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O10">
         <v>-7.4999999999999997E-2</v>
@@ -13116,22 +13116,22 @@
         <v>2.3205128205128198</v>
       </c>
       <c r="I11">
-        <v>0.143589743589743</v>
+        <v>-0.65641025641025597</v>
       </c>
       <c r="J11" s="1">
-        <v>-9.7435897435897395E-2</v>
+        <v>-1.6974358974358901</v>
       </c>
       <c r="K11" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L11" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M11" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N11" s="1">
-        <v>0.133333333333333</v>
+        <v>-1.4666666666666599</v>
       </c>
       <c r="O11">
         <v>0.7</v>
@@ -13175,25 +13175,25 @@
         <v>37</v>
       </c>
       <c r="H12">
-        <v>1.64358974358974</v>
+        <v>0.84358974358974304</v>
       </c>
       <c r="I12" s="1">
-        <v>0.107692307692307</v>
+        <v>-1.4923076923076899</v>
       </c>
       <c r="J12">
         <v>1.94871794871794</v>
       </c>
       <c r="K12" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="L12" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="M12" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N12" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="O12">
         <v>0.223232323232323</v>
@@ -13240,25 +13240,25 @@
         <v>38</v>
       </c>
       <c r="H13" s="1">
-        <v>1.1653846153846099</v>
+        <v>-0.43461538461538402</v>
       </c>
       <c r="I13" s="1">
-        <v>-6.9230769230769207E-2</v>
+        <v>-2.46923076923076</v>
       </c>
       <c r="J13">
         <v>2.4038461538461502</v>
       </c>
       <c r="K13" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="L13" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="M13" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N13" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -13305,22 +13305,22 @@
         <v>2.6858974358974299</v>
       </c>
       <c r="I14">
-        <v>0.83269230769230695</v>
+        <v>3.2692307692307597E-2</v>
       </c>
       <c r="J14" s="1">
-        <v>0.28141025641025602</v>
+        <v>-0.51858974358974297</v>
       </c>
       <c r="K14" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="L14" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="M14" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N14" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="O14">
         <v>0.7</v>
@@ -13367,22 +13367,22 @@
         <v>41</v>
       </c>
       <c r="H15">
-        <v>0.51904761904761898</v>
+        <v>-0.28095238095238001</v>
       </c>
       <c r="I15">
-        <v>-4.7619047619047701E-3</v>
+        <v>-0.80476190476190401</v>
       </c>
       <c r="J15">
-        <v>0.13809523809523799</v>
+        <v>-0.661904761904762</v>
       </c>
       <c r="K15">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L15">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M15">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N15">
         <v>1.0476190476190399</v>
@@ -13432,22 +13432,22 @@
         <v>4.2705128205128204</v>
       </c>
       <c r="I16" s="1">
-        <v>1.20192307692307</v>
+        <v>-1.1980769230769199</v>
       </c>
       <c r="J16" s="1">
-        <v>-0.17243589743589699</v>
+        <v>-3.3724358974358899</v>
       </c>
       <c r="K16" s="1">
-        <v>-0.6</v>
+        <v>-5.4</v>
       </c>
       <c r="L16" s="1">
-        <v>-0.6</v>
+        <v>-5.4</v>
       </c>
       <c r="M16" s="1">
-        <v>-0.6</v>
+        <v>-5.4</v>
       </c>
       <c r="N16" s="1">
-        <v>-0.6</v>
+        <v>-5.4</v>
       </c>
       <c r="O16">
         <v>0.7</v>
@@ -13497,22 +13497,22 @@
         <v>3.2805903189844199</v>
       </c>
       <c r="I17" s="1">
-        <v>0.413238573021181</v>
+        <v>-0.38676142697881799</v>
       </c>
       <c r="J17" s="1">
-        <v>-0.25652173913043402</v>
+        <v>-2.6565217391304299</v>
       </c>
       <c r="K17" s="1">
-        <v>-0.25652173913043402</v>
+        <v>-2.6565217391304299</v>
       </c>
       <c r="L17" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="M17" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N17" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="O17">
         <v>0.7</v>
@@ -13559,22 +13559,22 @@
         <v>1.82051282051282</v>
       </c>
       <c r="I18">
-        <v>-2.3076923076922998E-2</v>
+        <v>-0.82307692307692304</v>
       </c>
       <c r="J18">
-        <v>2.5641025641025498E-3</v>
+        <v>-0.79743589743589705</v>
       </c>
       <c r="K18">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L18">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M18">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N18">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -13618,25 +13618,25 @@
         <v>49</v>
       </c>
       <c r="H19">
-        <v>0.85824175824175797</v>
+        <v>5.8241758241758097E-2</v>
       </c>
       <c r="I19">
         <v>2.8879120879120799</v>
       </c>
       <c r="J19" s="1">
-        <v>-0.146153846153846</v>
+        <v>-2.5461538461538402</v>
       </c>
       <c r="K19" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="L19" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="M19" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N19" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="O19">
         <v>0.7</v>
@@ -13680,25 +13680,25 @@
         <v>50</v>
       </c>
       <c r="H20">
-        <v>0.515384615384615</v>
+        <v>-0.28461538461538399</v>
       </c>
       <c r="I20">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="J20">
         <v>1.3846153846153799</v>
       </c>
       <c r="K20">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L20">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M20">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N20">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O20">
         <v>0.1</v>
@@ -13746,22 +13746,22 @@
         <v>0.5</v>
       </c>
       <c r="I21" s="3">
-        <v>0.15</v>
+        <v>-0.65</v>
       </c>
       <c r="J21" s="3">
         <v>0.375</v>
       </c>
       <c r="K21" s="3">
-        <v>2.4999999999999901E-2</v>
+        <v>-0.77500000000000002</v>
       </c>
       <c r="L21" s="3">
-        <v>2.4999999999999901E-2</v>
+        <v>-0.77500000000000002</v>
       </c>
       <c r="M21" s="3">
         <v>0.375</v>
       </c>
       <c r="N21" s="3">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O21" s="3">
         <v>0.7</v>
@@ -13808,22 +13808,22 @@
         <v>1.82051282051282</v>
       </c>
       <c r="I22">
-        <v>-2.3076923076922998E-2</v>
+        <v>-0.82307692307692304</v>
       </c>
       <c r="J22">
-        <v>2.5641025641025498E-3</v>
+        <v>-0.79743589743589705</v>
       </c>
       <c r="K22">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L22">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M22">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N22">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O22">
         <v>0.7</v>
@@ -13870,22 +13870,22 @@
         <v>1.3653846153846101</v>
       </c>
       <c r="I23">
-        <v>0.15</v>
+        <v>-0.65</v>
       </c>
       <c r="J23">
-        <v>0.28461538461538399</v>
+        <v>-0.515384615384615</v>
       </c>
       <c r="K23">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L23">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M23">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N23">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O23">
         <v>0.24523809523809501</v>
@@ -13935,22 +13935,22 @@
         <v>1.9164598842018099</v>
       </c>
       <c r="I24">
-        <v>-4.8717948717948698E-2</v>
+        <v>-0.84871794871794803</v>
       </c>
       <c r="J24">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K24">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L24">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M24">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N24">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O24">
         <v>0.7</v>
@@ -13997,22 +13997,22 @@
         <v>3.4286908743430402</v>
       </c>
       <c r="I25" s="1">
-        <v>5.9117693900302498E-2</v>
+        <v>-1.5408823060996899</v>
       </c>
       <c r="J25" s="1">
-        <v>0.18413760152890499</v>
+        <v>-1.4158623984710901</v>
       </c>
       <c r="K25" s="1">
-        <v>-0.356521739130434</v>
+        <v>-3.5565217391304298</v>
       </c>
       <c r="L25" s="1">
-        <v>9.9999999999999895E-2</v>
+        <v>-3.1</v>
       </c>
       <c r="M25" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="N25" s="1">
-        <v>-2.3809523809523998E-3</v>
+        <v>-2.4023809523809501</v>
       </c>
       <c r="O25">
         <v>0.246428571428571</v>
@@ -14059,22 +14059,22 @@
         <v>4.3786908743430404</v>
       </c>
       <c r="I26" s="1">
-        <v>0.85911769390030202</v>
+        <v>-0.74088230609969696</v>
       </c>
       <c r="J26" s="1">
-        <v>8.41376015289058E-2</v>
+        <v>-2.31586239847109</v>
       </c>
       <c r="K26" s="1">
-        <v>-0.45652173913043398</v>
+        <v>-4.4565217391304301</v>
       </c>
       <c r="L26" s="1">
-        <v>-0.6</v>
+        <v>-5.4</v>
       </c>
       <c r="M26" s="1">
-        <v>-0.6</v>
+        <v>-5.4</v>
       </c>
       <c r="N26" s="1">
-        <v>-0.452380952380952</v>
+        <v>-4.4523809523809499</v>
       </c>
       <c r="O26">
         <v>0.35</v>
@@ -14121,22 +14121,22 @@
         <v>1.75</v>
       </c>
       <c r="I27" s="1">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="J27">
-        <v>0.15</v>
+        <v>-0.65</v>
       </c>
       <c r="K27" s="1">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L27" s="1">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M27" s="1">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N27" s="1">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O27">
         <v>0.28571428571428498</v>
@@ -14186,22 +14186,22 @@
         <v>2.3205128205128198</v>
       </c>
       <c r="I28">
-        <v>0.143589743589743</v>
+        <v>-0.65641025641025597</v>
       </c>
       <c r="J28" s="1">
-        <v>-9.7435897435897395E-2</v>
+        <v>-1.6974358974358901</v>
       </c>
       <c r="K28" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L28" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M28" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N28" s="1">
-        <v>0.133333333333333</v>
+        <v>-1.4666666666666599</v>
       </c>
       <c r="O28">
         <v>0.7</v>
@@ -14248,22 +14248,22 @@
         <v>2.5926102882624602</v>
       </c>
       <c r="I29" s="1">
-        <v>0.17743271221532</v>
+        <v>-0.62256728778467896</v>
       </c>
       <c r="J29">
         <v>0.90428412167542604</v>
       </c>
       <c r="K29" s="1">
-        <v>-0.25652173913043402</v>
+        <v>-2.6565217391304299</v>
       </c>
       <c r="L29" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="M29" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N29" s="1">
-        <v>-0.104761904761904</v>
+        <v>-1.7047619047619</v>
       </c>
       <c r="O29">
         <v>0.266666666666666</v>
@@ -14310,25 +14310,25 @@
         <v>67</v>
       </c>
       <c r="H30">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="I30">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="J30">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="K30">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L30">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="M30">
         <v>1</v>
       </c>
       <c r="N30">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O30">
         <v>0</v>
@@ -14378,19 +14378,19 @@
         <v>0.85714285714285698</v>
       </c>
       <c r="J31">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="K31">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L31">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="M31">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N31">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O31">
         <v>0</v>
@@ -14440,22 +14440,22 @@
         <v>1.7068723702664701</v>
       </c>
       <c r="I32">
-        <v>-1.30434782608695E-2</v>
+        <v>-0.81304347826086898</v>
       </c>
       <c r="J32">
-        <v>-5.6521739130434699E-2</v>
+        <v>-0.85652173913043395</v>
       </c>
       <c r="K32">
-        <v>-5.6521739130434699E-2</v>
+        <v>-0.85652173913043395</v>
       </c>
       <c r="L32">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M32">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N32">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O32">
         <v>0.7</v>
@@ -14499,25 +14499,25 @@
         <v>71</v>
       </c>
       <c r="H33" s="1">
-        <v>1.2891304347826</v>
+        <v>0.48913043478260798</v>
       </c>
       <c r="I33">
         <v>3.31195652173913</v>
       </c>
       <c r="J33" s="1">
-        <v>-0.131521739130434</v>
+        <v>-2.5315217391304299</v>
       </c>
       <c r="K33" s="1">
-        <v>-0.356521739130434</v>
+        <v>-3.5565217391304298</v>
       </c>
       <c r="L33" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="M33" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="N33" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="O33">
         <v>0.7</v>
@@ -14567,22 +14567,22 @@
         <v>1.9164598842018099</v>
       </c>
       <c r="I34">
-        <v>-4.8717948717948698E-2</v>
+        <v>-0.84871794871794803</v>
       </c>
       <c r="J34">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K34">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L34">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M34">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N34">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O34">
         <v>-0.2</v>
@@ -14629,22 +14629,22 @@
         <v>1.84615384615384</v>
       </c>
       <c r="I35">
-        <v>-6.9230769230769207E-2</v>
+        <v>-2.46923076923076</v>
       </c>
       <c r="J35">
         <v>1.92307692307692</v>
       </c>
       <c r="K35">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="L35">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="M35">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N35">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="O35">
         <v>0</v>
@@ -14694,19 +14694,19 @@
         <v>0.83333333333333304</v>
       </c>
       <c r="J36">
-        <v>0.15</v>
+        <v>-0.65</v>
       </c>
       <c r="K36">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L36">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M36">
-        <v>0.15</v>
+        <v>-0.65</v>
       </c>
       <c r="N36">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O36">
         <v>0.7</v>
@@ -14756,19 +14756,19 @@
         <v>0.54716117216117199</v>
       </c>
       <c r="J37">
-        <v>0.24065934065934</v>
+        <v>-0.55934065934065902</v>
       </c>
       <c r="K37" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L37" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M37" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N37" s="1">
-        <v>-0.15238095238095201</v>
+        <v>-1.7523809523809499</v>
       </c>
       <c r="O37">
         <v>0.15</v>
@@ -14818,22 +14818,22 @@
         <v>3.94725698565109</v>
       </c>
       <c r="I38" s="1">
-        <v>0.74657190635451498</v>
+        <v>-5.3428093645484898E-2</v>
       </c>
       <c r="J38" s="1">
-        <v>-0.356521739130434</v>
+        <v>-3.5565217391304298</v>
       </c>
       <c r="K38" s="1">
-        <v>-0.356521739130434</v>
+        <v>-3.5565217391304298</v>
       </c>
       <c r="L38" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="M38" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="N38" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="O38">
         <v>0.7</v>
@@ -14880,22 +14880,22 @@
         <v>1.82051282051282</v>
       </c>
       <c r="I39">
-        <v>-2.3076923076922998E-2</v>
+        <v>-0.82307692307692304</v>
       </c>
       <c r="J39">
-        <v>2.5641025641025498E-3</v>
+        <v>-0.79743589743589705</v>
       </c>
       <c r="K39">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L39">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M39">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N39">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O39">
         <v>0</v>
@@ -14939,25 +14939,25 @@
         <v>82</v>
       </c>
       <c r="H40">
-        <v>2.0034798534798499</v>
+        <v>1.2034798534798501</v>
       </c>
       <c r="I40" s="1">
-        <v>-0.109523809523809</v>
+        <v>-2.5095238095238002</v>
       </c>
       <c r="J40">
         <v>2.11080586080586</v>
       </c>
       <c r="K40" s="1">
-        <v>-0.15</v>
+        <v>-3.35</v>
       </c>
       <c r="L40" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="M40" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="N40" s="1">
-        <v>0.145238095238095</v>
+        <v>-1.4547619047619</v>
       </c>
       <c r="O40">
         <v>0.32499999999999901</v>
@@ -15007,19 +15007,19 @@
         <v>5.1282051282051197E-2</v>
       </c>
       <c r="J41">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="K41">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L41">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="M41">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N41">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O41">
         <v>0.5</v>
@@ -15066,22 +15066,22 @@
         <v>1.9164598842018099</v>
       </c>
       <c r="I42">
-        <v>-4.8717948717948698E-2</v>
+        <v>-0.84871794871794803</v>
       </c>
       <c r="J42">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K42">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L42">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M42">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N42">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O42">
         <v>0</v>
@@ -15243,25 +15243,25 @@
         <v>89</v>
       </c>
       <c r="H45">
-        <v>0.82307692307692304</v>
+        <v>2.3076923076923099E-2</v>
       </c>
       <c r="I45" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="J45">
         <v>2.07692307692307</v>
       </c>
       <c r="K45" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L45" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M45" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N45" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O45">
         <v>0.266666666666666</v>
@@ -15308,22 +15308,22 @@
         <v>1.82051282051282</v>
       </c>
       <c r="I46">
-        <v>-2.3076923076922998E-2</v>
+        <v>-0.82307692307692304</v>
       </c>
       <c r="J46">
-        <v>2.5641025641025498E-3</v>
+        <v>-0.79743589743589705</v>
       </c>
       <c r="K46" s="1">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L46" s="1">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M46" s="1">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N46" s="1">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O46">
         <v>0.34380952380952301</v>
@@ -15367,25 +15367,25 @@
         <v>91</v>
       </c>
       <c r="H47">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="I47">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="J47">
         <v>1.6666666666666601</v>
       </c>
       <c r="K47">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L47">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M47">
-        <v>0.233333333333333</v>
+        <v>-0.56666666666666599</v>
       </c>
       <c r="N47">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O47">
         <v>-0.15</v>
@@ -15432,22 +15432,22 @@
         <v>2.5414598842018199</v>
       </c>
       <c r="I48">
-        <v>0.32628205128205101</v>
+        <v>-0.47371794871794798</v>
       </c>
       <c r="J48" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="K48" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L48" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M48" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N48" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O48">
         <v>0.6</v>
@@ -15547,25 +15547,25 @@
         <v>97</v>
       </c>
       <c r="H50" s="1">
-        <v>0.53913043478260803</v>
+        <v>-1.0608695652173901</v>
       </c>
       <c r="I50" s="1">
-        <v>-0.113043478260869</v>
+        <v>-1.7130434782608599</v>
       </c>
       <c r="J50" s="1">
-        <v>-0.15652173913043399</v>
+        <v>-1.75652173913043</v>
       </c>
       <c r="K50">
         <v>1.5434782608695601</v>
       </c>
       <c r="L50" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M50" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N50" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O50">
         <v>0.35</v>
@@ -15612,22 +15612,22 @@
         <v>6.1891468746307403</v>
       </c>
       <c r="I51" s="1">
-        <v>7.3443223443223404E-2</v>
+        <v>-3.1265567765567699</v>
       </c>
       <c r="J51" s="1">
-        <v>0.57527472527472501</v>
+        <v>-2.6247252747252698</v>
       </c>
       <c r="K51" s="1">
-        <v>-0.79999999999999905</v>
+        <v>-7.2</v>
       </c>
       <c r="L51" s="1">
-        <v>-0.79999999999999905</v>
+        <v>-7.2</v>
       </c>
       <c r="M51" s="1">
-        <v>-0.44999999999999901</v>
+        <v>-6.05</v>
       </c>
       <c r="N51" s="1">
-        <v>-0.65238095238095195</v>
+        <v>-6.2523809523809497</v>
       </c>
       <c r="O51">
         <v>0</v>
@@ -15677,19 +15677,19 @@
         <v>0.28205128205128199</v>
       </c>
       <c r="J52">
-        <v>5.3846153846153801E-2</v>
+        <v>-0.74615384615384595</v>
       </c>
       <c r="K52">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L52">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M52">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N52">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O52">
         <v>0.7</v>
@@ -15736,22 +15736,22 @@
         <v>2.6555903189844199</v>
       </c>
       <c r="I53" s="1">
-        <v>3.82385730211817E-2</v>
+        <v>-0.76176142697881799</v>
       </c>
       <c r="J53" s="1">
-        <v>-0.15652173913043399</v>
+        <v>-1.75652173913043</v>
       </c>
       <c r="K53" s="1">
-        <v>-0.15652173913043399</v>
+        <v>-1.75652173913043</v>
       </c>
       <c r="L53" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M53" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N53" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O53">
         <v>0.44999999999999901</v>
@@ -15798,22 +15798,22 @@
         <v>1.9164598842018099</v>
       </c>
       <c r="I54">
-        <v>-4.8717948717948698E-2</v>
+        <v>-0.84871794871794803</v>
       </c>
       <c r="J54">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K54">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L54">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M54">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N54">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O54">
         <v>0</v>
@@ -15863,19 +15863,19 @@
         <v>5.1282051282051197E-2</v>
       </c>
       <c r="J55">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="K55">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L55">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="M55">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N55">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O55">
         <v>0.5</v>
@@ -15922,22 +15922,22 @@
         <v>2.4549214226633498</v>
       </c>
       <c r="I56" s="1">
-        <v>-0.148717948717948</v>
+        <v>-1.7487179487179401</v>
       </c>
       <c r="J56" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="K56" s="1">
-        <v>-4.6153846153846101E-2</v>
+        <v>-1.6461538461538401</v>
       </c>
       <c r="L56" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M56" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N56" s="1">
-        <v>0.107692307692307</v>
+        <v>-1.4923076923076899</v>
       </c>
       <c r="O56">
         <v>0</v>
@@ -15981,25 +15981,25 @@
         <v>106</v>
       </c>
       <c r="H57">
-        <v>1.0282051282051199</v>
+        <v>0.22820512820512801</v>
       </c>
       <c r="I57" s="1">
-        <v>-0.123076923076923</v>
+        <v>-1.7230769230769201</v>
       </c>
       <c r="J57">
         <v>1.79487179487179</v>
       </c>
       <c r="K57" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L57" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M57" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N57" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O57">
         <v>0.25833333333333303</v>
@@ -16043,25 +16043,25 @@
         <v>107</v>
       </c>
       <c r="H58">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="I58">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="J58">
         <v>1</v>
       </c>
       <c r="K58">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L58">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="M58">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N58">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O58">
         <v>0.7</v>
@@ -16169,22 +16169,22 @@
         <v>2.1025641025641</v>
       </c>
       <c r="I60">
-        <v>0.18205128205128199</v>
+        <v>-0.61794871794871797</v>
       </c>
       <c r="J60" s="1">
-        <v>-4.6153846153846101E-2</v>
+        <v>-1.6461538461538401</v>
       </c>
       <c r="K60" s="1">
-        <v>-4.6153846153846101E-2</v>
+        <v>-1.6461538461538401</v>
       </c>
       <c r="L60" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M60" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N60" s="1">
-        <v>0.107692307692307</v>
+        <v>-1.4923076923076899</v>
       </c>
       <c r="O60">
         <v>0.39999999999999902</v>
@@ -16231,22 +16231,22 @@
         <v>3.4164598842018199</v>
       </c>
       <c r="I61" s="1">
-        <v>-0.34871794871794798</v>
+        <v>-3.5487179487179401</v>
       </c>
       <c r="J61" s="1">
-        <v>7.4999999999999997E-2</v>
+        <v>-2.3250000000000002</v>
       </c>
       <c r="K61" s="1">
-        <v>7.4999999999999997E-2</v>
+        <v>-2.3250000000000002</v>
       </c>
       <c r="L61" s="1">
-        <v>-0.27500000000000002</v>
+        <v>-3.4750000000000001</v>
       </c>
       <c r="M61" s="1">
-        <v>-0.27500000000000002</v>
+        <v>-3.4750000000000001</v>
       </c>
       <c r="N61" s="1">
-        <v>-0.15</v>
+        <v>-3.35</v>
       </c>
       <c r="O61">
         <v>0.52499999999999902</v>
@@ -16349,25 +16349,25 @@
         <v>113</v>
       </c>
       <c r="H63">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="I63">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="J63">
         <v>1</v>
       </c>
       <c r="K63">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L63">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="M63">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N63">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O63">
         <v>-0.125</v>
@@ -16408,25 +16408,25 @@
         <v>114</v>
       </c>
       <c r="H64">
-        <v>1.32735042735042</v>
+        <v>0.52735042735042703</v>
       </c>
       <c r="I64" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="J64" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="K64">
         <v>1.3760683760683701</v>
       </c>
       <c r="L64" s="1">
-        <v>3.3333333333333201E-2</v>
+        <v>-2.36666666666666</v>
       </c>
       <c r="M64" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N64" s="1">
-        <v>0.429914529914529</v>
+        <v>-0.37008547008546999</v>
       </c>
       <c r="O64">
         <v>0.2</v>
@@ -16532,22 +16532,22 @@
         <v>2.4358974358974299</v>
       </c>
       <c r="I66">
-        <v>0.20769230769230701</v>
+        <v>-0.59230769230769198</v>
       </c>
       <c r="J66">
-        <v>0.15641025641025599</v>
+        <v>-0.64358974358974297</v>
       </c>
       <c r="K66" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L66" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M66" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N66" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O66">
         <v>0.21666666666666601</v>
@@ -16598,19 +16598,19 @@
         <v>1.0535714285714199</v>
       </c>
       <c r="J67" s="3">
-        <v>0.26309523809523799</v>
+        <v>-0.536904761904762</v>
       </c>
       <c r="K67" s="3">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L67" s="3">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M67" s="3">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N67" s="3">
-        <v>-0.15238095238095201</v>
+        <v>-1.7523809523809499</v>
       </c>
       <c r="O67" s="3">
         <v>0</v>
@@ -16657,22 +16657,22 @@
         <v>2.7476774433296098</v>
       </c>
       <c r="I68" s="1">
-        <v>0.269007803790412</v>
+        <v>-0.53099219620958704</v>
       </c>
       <c r="J68" s="1">
-        <v>-2.6755852842809398E-3</v>
+        <v>-1.60267558528428</v>
       </c>
       <c r="K68" s="1">
-        <v>0.28792270531400899</v>
+        <v>-1.31207729468599</v>
       </c>
       <c r="L68" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="M68" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N68" s="1">
-        <v>-0.188888888888888</v>
+        <v>-2.5888888888888801</v>
       </c>
       <c r="O68">
         <v>0.48</v>
@@ -16719,22 +16719,22 @@
         <v>4.6410256410256396</v>
       </c>
       <c r="I69" s="1">
-        <v>-0.146153846153846</v>
+        <v>-2.5461538461538402</v>
       </c>
       <c r="J69" s="1">
-        <v>-9.4871794871794896E-2</v>
+        <v>-2.49487179487179</v>
       </c>
       <c r="K69" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="L69" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="M69" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="N69" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="O69">
         <v>0.33076923076922998</v>
@@ -16781,22 +16781,22 @@
         <v>3.6858974358974299</v>
       </c>
       <c r="I70" s="1">
-        <v>0.95769230769230695</v>
+        <v>0.15769230769230699</v>
       </c>
       <c r="J70" s="1">
-        <v>-4.3589743589743601E-2</v>
+        <v>-2.4435897435897398</v>
       </c>
       <c r="K70" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="L70" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="M70" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="N70" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="O70">
         <v>0.7</v>
@@ -16840,25 +16840,25 @@
         <v>123</v>
       </c>
       <c r="H71" s="1">
-        <v>0.78290598290598201</v>
+        <v>-0.81709401709401697</v>
       </c>
       <c r="I71" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="J71" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="K71">
         <v>2.26495726495726</v>
       </c>
       <c r="L71" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="M71" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N71">
-        <v>0.65213675213675204</v>
+        <v>-0.147863247863247</v>
       </c>
       <c r="O71">
         <v>0.7</v>
@@ -16911,16 +16911,16 @@
         <v>0.43541965281095701</v>
       </c>
       <c r="K72" s="1">
-        <v>-0.15652173913043399</v>
+        <v>-1.75652173913043</v>
       </c>
       <c r="L72" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M72" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N72" s="1">
-        <v>-0.15238095238095201</v>
+        <v>-1.7523809523809499</v>
       </c>
       <c r="O72">
         <v>3.3333333333333298E-2</v>
@@ -16967,22 +16967,22 @@
         <v>2.02051282051282</v>
       </c>
       <c r="I73">
-        <v>0.77692307692307605</v>
+        <v>-2.3076923076922901E-2</v>
       </c>
       <c r="J73" s="1">
-        <v>-9.7435897435897395E-2</v>
+        <v>-1.6974358974358901</v>
       </c>
       <c r="K73" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L73" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M73" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N73" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O73">
         <v>0.39999999999999902</v>
@@ -17029,22 +17029,22 @@
         <v>1.9164598842018099</v>
       </c>
       <c r="I74">
-        <v>-4.8717948717948698E-2</v>
+        <v>-0.84871794871794803</v>
       </c>
       <c r="J74">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K74">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L74">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M74">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N74">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O74">
         <v>0.6</v>
@@ -17091,22 +17091,22 @@
         <v>1.82051282051282</v>
       </c>
       <c r="I75">
-        <v>-2.3076923076922998E-2</v>
+        <v>-0.82307692307692304</v>
       </c>
       <c r="J75">
-        <v>2.5641025641025498E-3</v>
+        <v>-0.79743589743589705</v>
       </c>
       <c r="K75">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L75">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M75">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N75">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O75">
         <v>0.35</v>
@@ -17150,25 +17150,25 @@
         <v>129</v>
       </c>
       <c r="H76">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="I76">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="J76">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="K76">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L76">
         <v>1</v>
       </c>
       <c r="M76">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N76">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O76">
         <v>0</v>
@@ -17215,22 +17215,22 @@
         <v>4.1536393713813</v>
       </c>
       <c r="I77" s="1">
-        <v>0.51153846153846105</v>
+        <v>-1.0884615384615299</v>
       </c>
       <c r="J77" s="1">
-        <v>-0.29743589743589699</v>
+        <v>-3.4974358974358899</v>
       </c>
       <c r="K77" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="L77" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="M77" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="N77" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="O77">
         <v>0</v>
@@ -17258,63 +17258,62 @@
       <c r="A78">
         <v>76</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" t="s">
         <v>131</v>
       </c>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3" t="s">
+      <c r="D78" t="s">
         <v>28</v>
       </c>
-      <c r="E78" s="3" t="s">
+      <c r="E78" t="s">
         <v>18</v>
       </c>
-      <c r="F78" s="3">
-        <v>0</v>
-      </c>
-      <c r="G78" s="3" t="s">
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78" t="s">
         <v>131</v>
       </c>
-      <c r="H78" s="3">
-        <v>1.6307692307692301</v>
-      </c>
-      <c r="I78" s="5">
-        <v>0.88653846153846105</v>
-      </c>
-      <c r="J78" s="3">
+      <c r="H78">
+        <v>0.83076923076923004</v>
+      </c>
+      <c r="I78">
+        <v>-0.71346153846153804</v>
+      </c>
+      <c r="J78">
         <v>1.5576923076922999</v>
       </c>
-      <c r="K78" s="5">
-        <v>-0.27500000000000002</v>
-      </c>
-      <c r="L78" s="5">
-        <v>-0.27500000000000002</v>
-      </c>
-      <c r="M78" s="5">
-        <v>-0.27500000000000002</v>
-      </c>
-      <c r="N78" s="5">
-        <v>-0.5</v>
-      </c>
-      <c r="O78" s="3">
+      <c r="K78" s="1">
+        <v>-3.4750000000000001</v>
+      </c>
+      <c r="L78" s="1">
+        <v>-3.4750000000000001</v>
+      </c>
+      <c r="M78" s="1">
+        <v>-3.4750000000000001</v>
+      </c>
+      <c r="N78" s="1">
+        <v>-4.5</v>
+      </c>
+      <c r="O78">
         <v>0.111837121212121</v>
       </c>
-      <c r="P78" s="3">
+      <c r="P78">
         <v>2.7027027027027001E-2</v>
       </c>
-      <c r="Q78" s="3">
+      <c r="Q78">
         <v>74</v>
       </c>
-      <c r="R78" s="3" t="str">
+      <c r="R78" t="str">
         <f t="shared" si="3"/>
-        <v>Jubilacion Patronal</v>
-      </c>
-      <c r="S78" s="3">
+        <v>IESS</v>
+      </c>
+      <c r="S78">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="T78" s="3">
+        <v>3</v>
+      </c>
+      <c r="T78">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.3">
@@ -17337,25 +17336,25 @@
         <v>132</v>
       </c>
       <c r="H79">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="I79">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="J79">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K79">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L79">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M79">
         <v>2</v>
       </c>
       <c r="N79">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O79">
         <v>0.5</v>
@@ -17402,22 +17401,22 @@
         <v>1.89743589743589</v>
       </c>
       <c r="I80">
-        <v>0.18205128205128199</v>
+        <v>-0.61794871794871797</v>
       </c>
       <c r="J80" s="1">
-        <v>-4.6153846153846101E-2</v>
+        <v>-1.6461538461538401</v>
       </c>
       <c r="K80" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L80" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M80" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N80" s="1">
-        <v>0.46666666666666601</v>
+        <v>-1.13333333333333</v>
       </c>
       <c r="O80">
         <v>0.27499999999999902</v>
@@ -17464,22 +17463,22 @@
         <v>1.8498168498168499</v>
       </c>
       <c r="I81">
-        <v>0.22600732600732601</v>
+        <v>-0.57399267399267395</v>
       </c>
       <c r="J81">
         <v>0.77655677655677602</v>
       </c>
       <c r="K81" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L81" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M81" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N81" s="1">
-        <v>-0.15238095238095201</v>
+        <v>-1.7523809523809499</v>
       </c>
       <c r="O81">
         <v>0</v>
@@ -17523,22 +17522,22 @@
         <v>0.2</v>
       </c>
       <c r="I82">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="J82">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="K82">
         <v>0.8</v>
       </c>
       <c r="L82">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="M82">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N82">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O82">
         <v>0.7</v>
@@ -17582,22 +17581,22 @@
         <v>137</v>
       </c>
       <c r="H83" s="1">
-        <v>1.1162393162393101</v>
+        <v>-0.48376068376068299</v>
       </c>
       <c r="I83" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="J83" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="K83" s="1">
-        <v>1.0649572649572601</v>
+        <v>-0.53504273504273503</v>
       </c>
       <c r="L83" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="M83" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="N83">
         <v>2.4188034188034102</v>
@@ -17647,22 +17646,22 @@
         <v>3.8936855570796598</v>
       </c>
       <c r="I84" s="1">
-        <v>0.22871476349737199</v>
+        <v>-0.57128523650262697</v>
       </c>
       <c r="J84" s="1">
-        <v>0.31966873706004101</v>
+        <v>-1.2803312629399499</v>
       </c>
       <c r="K84" s="1">
-        <v>-0.356521739130434</v>
+        <v>-3.5565217391304298</v>
       </c>
       <c r="L84" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="M84" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="N84" s="1">
-        <v>-0.20476190476190401</v>
+        <v>-2.6047619047618999</v>
       </c>
       <c r="O84">
         <v>0</v>
@@ -17706,25 +17705,25 @@
         <v>140</v>
       </c>
       <c r="H85" s="1">
-        <v>4.9999999999999899E-2</v>
+        <v>-1.55</v>
       </c>
       <c r="I85" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="J85" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="K85" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L85">
         <v>2.5</v>
       </c>
       <c r="M85" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N85" s="1">
-        <v>4.9999999999999899E-2</v>
+        <v>-1.55</v>
       </c>
       <c r="O85">
         <v>0</v>
@@ -17771,22 +17770,22 @@
         <v>3.4358974358974299</v>
       </c>
       <c r="I86" s="1">
-        <v>0.107692307692307</v>
+        <v>-1.4923076923076899</v>
       </c>
       <c r="J86" s="1">
-        <v>5.6410256410256397E-2</v>
+        <v>-1.5435897435897401</v>
       </c>
       <c r="K86" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="L86" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="M86" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N86" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="O86">
         <v>0.44999999999999901</v>
@@ -17836,19 +17835,19 @@
         <v>0.138238573021181</v>
       </c>
       <c r="J87">
-        <v>-5.6521739130434699E-2</v>
+        <v>-0.85652173913043395</v>
       </c>
       <c r="K87">
-        <v>-5.6521739130434699E-2</v>
+        <v>-0.85652173913043395</v>
       </c>
       <c r="L87">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M87">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N87">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O87">
         <v>0.7</v>
@@ -17898,19 +17897,19 @@
         <v>1.1734949832775901</v>
       </c>
       <c r="J88" s="1">
-        <v>-0.15395763656633199</v>
+        <v>-2.5539576365663299</v>
       </c>
       <c r="K88" s="1">
-        <v>-0.356521739130434</v>
+        <v>-3.5565217391304298</v>
       </c>
       <c r="L88" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="M88" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="N88" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="O88">
         <v>0</v>
@@ -17961,19 +17960,19 @@
         <v>1.1734949832775901</v>
       </c>
       <c r="J89" s="7">
-        <v>-0.15395763656633199</v>
+        <v>-2.5539576365663299</v>
       </c>
       <c r="K89" s="7">
-        <v>-0.356521739130434</v>
+        <v>-3.5565217391304298</v>
       </c>
       <c r="L89" s="7">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="M89" s="7">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="N89" s="7">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="O89" s="6">
         <v>0</v>
@@ -18023,19 +18022,19 @@
         <v>1.1071428571428501</v>
       </c>
       <c r="J90">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K90">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L90">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M90">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N90">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O90">
         <v>0.266666666666666</v>
@@ -18085,19 +18084,19 @@
         <v>1.6571428571428499</v>
       </c>
       <c r="J91">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K91">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L91">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M91">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N91">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O91">
         <v>0.2</v>
@@ -18144,19 +18143,19 @@
         <v>0.25</v>
       </c>
       <c r="I92">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="J92">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="K92">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L92">
         <v>0.5</v>
       </c>
       <c r="M92">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N92">
         <v>0.25</v>
@@ -18206,22 +18205,22 @@
         <v>1.9164598842018099</v>
       </c>
       <c r="I93">
-        <v>-4.8717948717948698E-2</v>
+        <v>-0.84871794871794803</v>
       </c>
       <c r="J93">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K93">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L93">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M93">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N93">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O93">
         <v>0</v>
@@ -18259,25 +18258,25 @@
         <v>149</v>
       </c>
       <c r="H94" s="1">
-        <v>0.24444444444444399</v>
+        <v>-1.3555555555555501</v>
       </c>
       <c r="I94" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="J94" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="K94">
         <v>2.1111111111111098</v>
       </c>
       <c r="L94" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M94" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N94">
-        <v>0.344444444444444</v>
+        <v>-0.45555555555555499</v>
       </c>
       <c r="O94">
         <v>0.7</v>
@@ -18324,22 +18323,22 @@
         <v>2.5384615384615299</v>
       </c>
       <c r="I95" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="J95" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="K95" s="1">
-        <v>-4.6153846153846101E-2</v>
+        <v>-1.6461538461538401</v>
       </c>
       <c r="L95" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M95" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N95" s="1">
-        <v>0.107692307692307</v>
+        <v>-1.4923076923076899</v>
       </c>
       <c r="O95">
         <v>0</v>
@@ -18386,22 +18385,22 @@
         <v>1.9164598842018099</v>
       </c>
       <c r="I96">
-        <v>-4.8717948717948698E-2</v>
+        <v>-0.84871794871794803</v>
       </c>
       <c r="J96">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K96">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L96">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M96">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N96">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O96">
         <v>0.47499999999999998</v>
@@ -18448,22 +18447,22 @@
         <v>2.6555903189844199</v>
       </c>
       <c r="I97" s="1">
-        <v>3.82385730211817E-2</v>
+        <v>-0.76176142697881799</v>
       </c>
       <c r="J97" s="1">
-        <v>-0.15652173913043399</v>
+        <v>-1.75652173913043</v>
       </c>
       <c r="K97" s="1">
-        <v>-0.15652173913043399</v>
+        <v>-1.75652173913043</v>
       </c>
       <c r="L97" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M97" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N97" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O97">
         <v>0.7</v>
@@ -18501,25 +18500,25 @@
         <v>155</v>
       </c>
       <c r="H98" s="1">
-        <v>0.75</v>
+        <v>-0.85</v>
       </c>
       <c r="I98" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="J98" s="1">
-        <v>-0.15</v>
+        <v>-3.35</v>
       </c>
       <c r="K98">
         <v>3.55</v>
       </c>
       <c r="L98" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="M98" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="N98" s="1">
-        <v>-0.15</v>
+        <v>-3.35</v>
       </c>
       <c r="O98">
         <v>0</v>
@@ -18625,22 +18624,22 @@
         <v>1.1428571428571399</v>
       </c>
       <c r="I100">
-        <v>0.75714285714285701</v>
+        <v>-4.2857142857142899E-2</v>
       </c>
       <c r="J100">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K100">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L100">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M100">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N100">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O100">
         <v>0.7</v>
@@ -18687,22 +18686,22 @@
         <v>1.66220735785953</v>
       </c>
       <c r="I101">
-        <v>-0.213043478260869</v>
+        <v>-2.61304347826086</v>
       </c>
       <c r="J101">
         <v>2.1204013377926398</v>
       </c>
       <c r="K101">
-        <v>-0.25652173913043402</v>
+        <v>-2.6565217391304299</v>
       </c>
       <c r="L101">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="M101">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N101">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="O101">
         <v>6.1111111111111102E-2</v>
@@ -18746,25 +18745,25 @@
         <v>160</v>
       </c>
       <c r="H102">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="I102">
         <v>2</v>
       </c>
       <c r="J102">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K102">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L102">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M102">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N102">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O102">
         <v>0</v>
@@ -18811,22 +18810,22 @@
         <v>1.57051282051282</v>
       </c>
       <c r="I103">
-        <v>-2.3076923076922998E-2</v>
+        <v>-0.82307692307692304</v>
       </c>
       <c r="J103">
         <v>0.35256410256410198</v>
       </c>
       <c r="K103">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L103">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M103">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N103">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O103">
         <v>0.149999999999999</v>
@@ -18870,25 +18869,25 @@
         <v>163</v>
       </c>
       <c r="H104">
-        <v>0.86190476190476195</v>
+        <v>6.19047619047619E-2</v>
       </c>
       <c r="I104">
         <v>2.7523809523809502</v>
       </c>
       <c r="J104" s="1">
-        <v>-6.19047619047619E-2</v>
+        <v>-2.4619047619047598</v>
       </c>
       <c r="K104" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="L104" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="M104" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N104" s="1">
-        <v>-0.25238095238095198</v>
+        <v>-2.6523809523809501</v>
       </c>
       <c r="O104">
         <v>0.3</v>
@@ -19050,25 +19049,25 @@
         <v>166</v>
       </c>
       <c r="H107">
-        <v>0.15</v>
+        <v>-0.65</v>
       </c>
       <c r="I107">
-        <v>0.15</v>
+        <v>-0.65</v>
       </c>
       <c r="J107">
         <v>1.25</v>
       </c>
       <c r="K107">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L107">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M107">
-        <v>0.15</v>
+        <v>-0.65</v>
       </c>
       <c r="N107">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O107">
         <v>0</v>
@@ -19106,25 +19105,25 @@
         <v>167</v>
       </c>
       <c r="H108">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="I108">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="J108">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K108">
         <v>2</v>
       </c>
       <c r="L108">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M108">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N108">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O108">
         <v>0.7</v>
@@ -19227,22 +19226,22 @@
         <v>3.32225698565109</v>
       </c>
       <c r="I110" s="1">
-        <v>0.37157190635451498</v>
+        <v>-0.42842809364548401</v>
       </c>
       <c r="J110" s="1">
-        <v>-0.25652173913043402</v>
+        <v>-2.6565217391304299</v>
       </c>
       <c r="K110" s="1">
-        <v>-0.25652173913043402</v>
+        <v>-2.6565217391304299</v>
       </c>
       <c r="L110" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="M110" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N110" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="O110">
         <v>0</v>
@@ -19345,22 +19344,22 @@
         <v>2.4358974358974299</v>
       </c>
       <c r="I112">
-        <v>0.20769230769230701</v>
+        <v>-0.59230769230769198</v>
       </c>
       <c r="J112">
-        <v>0.15641025641025599</v>
+        <v>-0.64358974358974297</v>
       </c>
       <c r="K112" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L112" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M112" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N112" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O112">
         <v>0</v>
@@ -19407,22 +19406,22 @@
         <v>2.7497932175351498</v>
       </c>
       <c r="I113" s="1">
-        <v>0.117948717948717</v>
+        <v>-0.68205128205128196</v>
       </c>
       <c r="J113" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="K113" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L113" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M113" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N113" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O113">
         <v>0.35</v>
@@ -19528,22 +19527,22 @@
         <v>1.9164598842018099</v>
       </c>
       <c r="I115">
-        <v>-4.8717948717948698E-2</v>
+        <v>-0.84871794871794803</v>
       </c>
       <c r="J115">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K115">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L115">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M115">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N115">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O115">
         <v>0</v>
@@ -19587,25 +19586,25 @@
         <v>177</v>
       </c>
       <c r="H116" s="1">
-        <v>1.0344322344322301</v>
+        <v>-0.565567765567765</v>
       </c>
       <c r="I116" s="1">
-        <v>-0.20476190476190401</v>
+        <v>-2.6047619047618999</v>
       </c>
       <c r="J116">
         <v>2.6227106227106201</v>
       </c>
       <c r="K116" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="L116" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="M116" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N116" s="1">
-        <v>-0.25238095238095198</v>
+        <v>-2.6523809523809501</v>
       </c>
       <c r="O116">
         <v>0.44999999999999901</v>
@@ -19771,22 +19770,22 @@
         <v>2.4358974358974299</v>
       </c>
       <c r="I119">
-        <v>0.20769230769230701</v>
+        <v>-0.59230769230769198</v>
       </c>
       <c r="J119">
-        <v>0.15641025641025599</v>
+        <v>-0.64358974358974297</v>
       </c>
       <c r="K119" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L119" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M119" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N119" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O119">
         <v>0.7</v>
@@ -19833,22 +19832,22 @@
         <v>1.85347985347985</v>
       </c>
       <c r="I120">
-        <v>9.0476190476190405E-2</v>
+        <v>-0.709523809523809</v>
       </c>
       <c r="J120">
         <v>0.86080586080585997</v>
       </c>
       <c r="K120">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L120">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M120">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N120">
-        <v>-4.7619047619047701E-3</v>
+        <v>-0.80476190476190401</v>
       </c>
       <c r="O120">
         <v>0</v>
@@ -19891,25 +19890,25 @@
         <v>184</v>
       </c>
       <c r="H121" s="3">
-        <v>0.639130434782608</v>
+        <v>-0.16086956521739099</v>
       </c>
       <c r="I121" s="3">
-        <v>-1.30434782608695E-2</v>
+        <v>-0.81304347826086898</v>
       </c>
       <c r="J121" s="3">
-        <v>-5.6521739130434699E-2</v>
+        <v>-0.85652173913043395</v>
       </c>
       <c r="K121" s="3">
-        <v>-5.6521739130434699E-2</v>
+        <v>-0.85652173913043395</v>
       </c>
       <c r="L121" s="3">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M121" s="3">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N121" s="3">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O121" s="3">
         <v>0.36666666666666597</v>
@@ -19959,19 +19958,19 @@
         <v>0.8</v>
       </c>
       <c r="J122">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="K122">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L122">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="M122">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N122">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O122">
         <v>0</v>
@@ -20018,22 +20017,22 @@
         <v>2.2371794871794801</v>
       </c>
       <c r="I123">
-        <v>0.56025641025641004</v>
+        <v>-0.239743589743589</v>
       </c>
       <c r="J123" s="1">
-        <v>-9.7435897435897395E-2</v>
+        <v>-1.6974358974358901</v>
       </c>
       <c r="K123" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L123" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M123" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N123" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O123">
         <v>0.35</v>
@@ -20136,22 +20135,22 @@
         <v>1.67307692307692</v>
       </c>
       <c r="I125" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="J125">
         <v>1.32692307692307</v>
       </c>
       <c r="K125" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L125" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M125" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N125" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O125">
         <v>0.39999999999999902</v>
@@ -20195,25 +20194,25 @@
         <v>190</v>
       </c>
       <c r="H126">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="I126">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="J126">
         <v>2</v>
       </c>
       <c r="K126">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L126">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M126">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N126">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O126">
         <v>0</v>
@@ -20260,22 +20259,22 @@
         <v>3.2709749343690402</v>
       </c>
       <c r="I127" s="1">
-        <v>-6.1761426978818298E-2</v>
+        <v>-1.6617614269788099</v>
       </c>
       <c r="J127" s="1">
-        <v>0.22809364548494901</v>
+        <v>-1.3719063545150501</v>
       </c>
       <c r="K127" s="1">
-        <v>-0.25652173913043402</v>
+        <v>-2.6565217391304299</v>
       </c>
       <c r="L127" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="M127" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N127" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="O127">
         <v>0.25</v>
@@ -20303,63 +20302,62 @@
       <c r="A128">
         <v>126</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="B128" t="s">
         <v>193</v>
       </c>
-      <c r="C128" s="4"/>
-      <c r="D128" s="3" t="s">
+      <c r="D128" t="s">
         <v>17</v>
       </c>
-      <c r="E128" s="3" t="s">
+      <c r="E128" t="s">
         <v>18</v>
       </c>
-      <c r="F128" s="3">
-        <v>0</v>
-      </c>
-      <c r="G128" s="3" t="s">
+      <c r="F128">
+        <v>0</v>
+      </c>
+      <c r="G128" t="s">
         <v>194</v>
       </c>
-      <c r="H128" s="3">
-        <v>3.30961538461538</v>
-      </c>
-      <c r="I128" s="3">
+      <c r="H128">
+        <v>2.5096153846153801</v>
+      </c>
+      <c r="I128" s="1">
         <v>2.8339743589743498</v>
       </c>
-      <c r="J128" s="5">
-        <v>-0.243589743589743</v>
-      </c>
-      <c r="K128" s="5">
-        <v>-0.7</v>
-      </c>
-      <c r="L128" s="5">
-        <v>-0.7</v>
-      </c>
-      <c r="M128" s="5">
-        <v>-0.1</v>
-      </c>
-      <c r="N128" s="5">
-        <v>-0.7</v>
-      </c>
-      <c r="O128" s="3">
+      <c r="J128" s="1">
+        <v>-4.2435897435897401</v>
+      </c>
+      <c r="K128" s="1">
+        <v>-6.3</v>
+      </c>
+      <c r="L128" s="1">
+        <v>-6.3</v>
+      </c>
+      <c r="M128" s="1">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="N128" s="1">
+        <v>-6.3</v>
+      </c>
+      <c r="O128">
         <v>9.5833333333333298E-2</v>
       </c>
-      <c r="P128" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q128" s="3">
+      <c r="P128">
+        <v>0</v>
+      </c>
+      <c r="Q128">
         <v>49</v>
       </c>
-      <c r="R128" s="3" t="str">
+      <c r="R128" t="str">
         <f t="shared" si="3"/>
-        <v>Jubilacion Patronal</v>
-      </c>
-      <c r="S128" s="3">
+        <v>Renuncia/Despido/Desahucio</v>
+      </c>
+      <c r="S128">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="T128" s="3">
+        <v>2</v>
+      </c>
+      <c r="T128">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:20" x14ac:dyDescent="0.3">
@@ -20444,22 +20442,22 @@
         <v>2.88420181968569</v>
       </c>
       <c r="I130" s="1">
-        <v>-0.148717948717948</v>
+        <v>-1.7487179487179401</v>
       </c>
       <c r="J130" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="K130" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L130" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M130" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N130" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O130">
         <v>0.2</v>
@@ -20503,25 +20501,25 @@
         <v>197</v>
       </c>
       <c r="H131">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="I131">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="J131">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="K131">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L131">
         <v>1</v>
       </c>
       <c r="M131">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N131">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O131">
         <v>0</v>
@@ -20568,22 +20566,22 @@
         <v>1.9164598842018099</v>
       </c>
       <c r="I132">
-        <v>-4.8717948717948698E-2</v>
+        <v>-0.84871794871794803</v>
       </c>
       <c r="J132">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K132">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L132">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M132">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N132">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O132">
         <v>0.1</v>
@@ -20627,25 +20625,25 @@
         <v>199</v>
       </c>
       <c r="H133">
-        <v>0.31666666666666599</v>
+        <v>-0.483333333333333</v>
       </c>
       <c r="I133">
         <v>1.5833333333333299</v>
       </c>
       <c r="J133">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K133">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L133">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M133">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N133">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O133">
         <v>0</v>
@@ -20695,19 +20693,19 @@
         <v>1.03076923076923</v>
       </c>
       <c r="J134">
-        <v>5.3846153846153801E-2</v>
+        <v>-0.74615384615384595</v>
       </c>
       <c r="K134">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L134">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M134">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N134">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O134">
         <v>0.33333333333333298</v>
@@ -20754,22 +20752,22 @@
         <v>1.9164598842018099</v>
       </c>
       <c r="I135">
-        <v>-4.8717948717948698E-2</v>
+        <v>-0.84871794871794803</v>
       </c>
       <c r="J135">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K135">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L135">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M135">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N135">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O135">
         <v>0.7</v>
@@ -20813,25 +20811,25 @@
         <v>203</v>
       </c>
       <c r="H136">
-        <v>0.31666666666666599</v>
+        <v>-0.483333333333333</v>
       </c>
       <c r="I136">
         <v>1.5833333333333299</v>
       </c>
       <c r="J136">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K136">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L136">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M136">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N136">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O136">
         <v>0</v>
@@ -20881,19 +20879,19 @@
         <v>0.82692307692307698</v>
       </c>
       <c r="J137" s="1">
-        <v>-9.7435897435897395E-2</v>
+        <v>-1.6974358974358901</v>
       </c>
       <c r="K137" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L137" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M137" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N137" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O137">
         <v>0.7</v>
@@ -20944,19 +20942,19 @@
         <v>0.82692307692307698</v>
       </c>
       <c r="J138" s="7">
-        <v>-9.7435897435897395E-2</v>
+        <v>-1.6974358974358901</v>
       </c>
       <c r="K138" s="7">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L138" s="7">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M138" s="7">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N138" s="7">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O138" s="6">
         <v>0.7</v>
@@ -21006,19 +21004,19 @@
         <v>0.44047619047619002</v>
       </c>
       <c r="J139">
-        <v>0.37619047619047602</v>
+        <v>-0.42380952380952303</v>
       </c>
       <c r="K139" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L139" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M139" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N139" s="1">
-        <v>-4.7619047619047701E-3</v>
+        <v>-0.80476190476190401</v>
       </c>
       <c r="O139">
         <v>0.10222222222222201</v>
@@ -21056,25 +21054,25 @@
         <v>206</v>
       </c>
       <c r="H140">
-        <v>0.1</v>
+        <v>-0.7</v>
       </c>
       <c r="I140">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="J140">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K140">
         <v>1.8</v>
       </c>
       <c r="L140">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M140">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N140">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O140">
         <v>0</v>
@@ -21112,25 +21110,25 @@
         <v>207</v>
       </c>
       <c r="H141">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="I141">
-        <v>0.4</v>
+        <v>-0.4</v>
       </c>
       <c r="J141">
-        <v>0.56666666666666599</v>
+        <v>-0.233333333333333</v>
       </c>
       <c r="K141">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L141">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M141">
         <v>0.83333333333333304</v>
       </c>
       <c r="N141">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O141">
         <v>0</v>
@@ -21174,25 +21172,25 @@
         <v>208</v>
       </c>
       <c r="H142">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="I142">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="J142">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="K142">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L142">
         <v>1</v>
       </c>
       <c r="M142">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N142">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O142">
         <v>0</v>
@@ -21239,22 +21237,22 @@
         <v>3.1164598842018201</v>
       </c>
       <c r="I143" s="1">
-        <v>-0.34871794871794798</v>
+        <v>-3.5487179487179401</v>
       </c>
       <c r="J143" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="K143" s="1">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="L143" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="M143" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="N143" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="O143">
         <v>0.25</v>
@@ -21302,22 +21300,22 @@
         <v>3.2451159951159898</v>
       </c>
       <c r="I144" s="1">
-        <v>-0.25347985347985302</v>
+        <v>-3.4534798534798501</v>
       </c>
       <c r="J144" s="1">
-        <v>-3.6904761904761899E-2</v>
+        <v>-3.2369047619047602</v>
       </c>
       <c r="K144" s="1">
-        <v>0.96773504273504196</v>
+        <v>-0.63226495726495702</v>
       </c>
       <c r="L144" s="1">
-        <v>-0.375</v>
+        <v>-4.375</v>
       </c>
       <c r="M144" s="1">
-        <v>-0.375</v>
+        <v>-4.375</v>
       </c>
       <c r="N144" s="1">
-        <v>0.37753357753357702</v>
+        <v>-1.2224664224664199</v>
       </c>
       <c r="O144">
         <v>0</v>
@@ -21364,22 +21362,22 @@
         <v>2.5128205128205101</v>
       </c>
       <c r="I145" s="1">
-        <v>0.107692307692307</v>
+        <v>-1.4923076923076899</v>
       </c>
       <c r="J145" s="1">
-        <v>5.6410256410256397E-2</v>
+        <v>-1.5435897435897401</v>
       </c>
       <c r="K145" s="1">
-        <v>0.107692307692307</v>
+        <v>-1.4923076923076899</v>
       </c>
       <c r="L145" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="M145" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N145" s="1">
-        <v>0.41538461538461502</v>
+        <v>-1.18461538461538</v>
       </c>
       <c r="O145">
         <v>0.233333333333333</v>
@@ -21429,19 +21427,19 @@
         <v>1.6141025641025599</v>
       </c>
       <c r="J146" s="1">
-        <v>-4.6153846153846101E-2</v>
+        <v>-1.6461538461538401</v>
       </c>
       <c r="K146" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L146" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M146" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N146" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O146">
         <v>0.7</v>
@@ -21488,22 +21486,22 @@
         <v>2.6555903189844199</v>
       </c>
       <c r="I147" s="1">
-        <v>3.82385730211817E-2</v>
+        <v>-0.76176142697881799</v>
       </c>
       <c r="J147" s="1">
-        <v>-0.15652173913043399</v>
+        <v>-1.75652173913043</v>
       </c>
       <c r="K147" s="1">
-        <v>-0.15652173913043399</v>
+        <v>-1.75652173913043</v>
       </c>
       <c r="L147" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M147" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N147" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O147">
         <v>0.7</v>
@@ -21603,25 +21601,25 @@
         <v>216</v>
       </c>
       <c r="H149">
-        <v>1.59038461538461</v>
+        <v>0.79038461538461502</v>
       </c>
       <c r="I149">
         <v>3.0307692307692302</v>
       </c>
       <c r="J149" s="1">
-        <v>-2.11538461538461E-2</v>
+        <v>-2.4211538461538402</v>
       </c>
       <c r="K149" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="L149" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="M149" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="N149" s="1">
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="O149">
         <v>0.7</v>
@@ -21669,22 +21667,22 @@
         <v>1.9164598842018099</v>
       </c>
       <c r="I150">
-        <v>-4.8717948717948698E-2</v>
+        <v>-0.84871794871794803</v>
       </c>
       <c r="J150">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K150">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L150">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M150">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N150">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O150">
         <v>0.43333333333333302</v>
@@ -21731,22 +21729,22 @@
         <v>2.5641025641025599</v>
       </c>
       <c r="I151">
-        <v>0.18205128205128199</v>
+        <v>-0.61794871794871797</v>
       </c>
       <c r="J151" s="1">
-        <v>-4.6153846153846101E-2</v>
+        <v>-1.6461538461538401</v>
       </c>
       <c r="K151" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L151" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M151" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N151" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O151">
         <v>0.35</v>
@@ -21784,22 +21782,22 @@
         <v>220</v>
       </c>
       <c r="H152">
-        <v>0.77179487179487105</v>
+        <v>-2.8205128205128199E-2</v>
       </c>
       <c r="I152" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="J152" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="K152" s="1">
-        <v>-4.6153846153846101E-2</v>
+        <v>-1.6461538461538401</v>
       </c>
       <c r="L152" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M152" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N152">
         <v>1.97435897435897</v>
@@ -21846,25 +21844,25 @@
         <v>221</v>
       </c>
       <c r="H153" s="1">
-        <v>4.9999999999999899E-2</v>
+        <v>-1.55</v>
       </c>
       <c r="I153">
         <v>2.625</v>
       </c>
       <c r="J153" s="1">
-        <v>-7.4999999999999997E-2</v>
+        <v>-1.675</v>
       </c>
       <c r="K153" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="L153" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M153" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N153" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="O153">
         <v>0.2</v>
@@ -21974,19 +21972,19 @@
         <v>0.25</v>
       </c>
       <c r="J155">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="K155">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L155">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="M155">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N155">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O155">
         <v>0.16666666666666599</v>
@@ -22034,22 +22032,22 @@
         <v>1.7692307692307601</v>
       </c>
       <c r="I156" s="1">
-        <v>3.0769230769230702E-2</v>
+        <v>-1.5692307692307601</v>
       </c>
       <c r="J156">
-        <v>0.43846153846153801</v>
+        <v>-0.36153846153846098</v>
       </c>
       <c r="K156" s="1">
-        <v>-4.6153846153846101E-2</v>
+        <v>-1.6461538461538401</v>
       </c>
       <c r="L156" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="M156" s="1">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="N156" s="1">
-        <v>0.107692307692307</v>
+        <v>-1.4923076923076899</v>
       </c>
       <c r="O156">
         <v>0</v>
@@ -22090,22 +22088,22 @@
         <v>0.7</v>
       </c>
       <c r="I157">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="J157">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K157">
         <v>1.3</v>
       </c>
       <c r="L157">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M157">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N157">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O157">
         <v>0.7</v>
@@ -22208,25 +22206,25 @@
         <v>230</v>
       </c>
       <c r="H159">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="I159">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="J159">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K159">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L159">
         <v>2</v>
       </c>
       <c r="M159">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N159">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O159">
         <v>0.25312499999999999</v>
@@ -22270,25 +22268,25 @@
         <v>232</v>
       </c>
       <c r="H160">
-        <v>0.15</v>
+        <v>-0.65</v>
       </c>
       <c r="I160">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="J160">
-        <v>2.4999999999999901E-2</v>
+        <v>-0.77500000000000002</v>
       </c>
       <c r="K160">
-        <v>2.4999999999999901E-2</v>
+        <v>-0.77500000000000002</v>
       </c>
       <c r="L160">
         <v>1.125</v>
       </c>
       <c r="M160">
-        <v>2.4999999999999901E-2</v>
+        <v>-0.77500000000000002</v>
       </c>
       <c r="N160">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O160">
         <v>0.3</v>
@@ -22332,19 +22330,19 @@
         <v>0.91666666666666596</v>
       </c>
       <c r="I161" s="3">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="J161" s="3">
-        <v>0.15</v>
+        <v>-0.65</v>
       </c>
       <c r="K161" s="3">
-        <v>0.15</v>
+        <v>-0.65</v>
       </c>
       <c r="L161" s="3">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M161" s="3">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N161" s="3">
         <v>0.58333333333333304</v>
@@ -22447,25 +22445,25 @@
         <v>235</v>
       </c>
       <c r="H163">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="I163">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="J163">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="K163">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L163">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="M163">
         <v>1</v>
       </c>
       <c r="N163">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O163">
         <v>0</v>
@@ -22503,25 +22501,25 @@
         <v>236</v>
       </c>
       <c r="H164">
-        <v>0.15</v>
+        <v>-0.65</v>
       </c>
       <c r="I164">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="J164">
-        <v>2.4999999999999901E-2</v>
+        <v>-0.77500000000000002</v>
       </c>
       <c r="K164">
         <v>1.125</v>
       </c>
       <c r="L164">
-        <v>2.4999999999999901E-2</v>
+        <v>-0.77500000000000002</v>
       </c>
       <c r="M164">
-        <v>2.4999999999999901E-2</v>
+        <v>-0.77500000000000002</v>
       </c>
       <c r="N164">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O164">
         <v>0</v>
@@ -22562,25 +22560,25 @@
         <v>237</v>
       </c>
       <c r="H165">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="I165">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="J165">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K165">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L165">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M165">
         <v>2</v>
       </c>
       <c r="N165">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O165">
         <v>0.1</v>
@@ -22738,22 +22736,22 @@
         <v>240</v>
       </c>
       <c r="H168" s="1">
-        <v>0.58846153846153804</v>
+        <v>-1.0115384615384599</v>
       </c>
       <c r="I168" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="J168" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="K168" s="1">
-        <v>-0.146153846153846</v>
+        <v>-2.5461538461538402</v>
       </c>
       <c r="L168" s="1">
-        <v>0.19999999999999901</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="M168" s="1">
-        <v>-0.4</v>
+        <v>-3.6</v>
       </c>
       <c r="N168">
         <v>2.5576923076922999</v>
@@ -22797,25 +22795,25 @@
         <v>241</v>
       </c>
       <c r="H169">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="I169">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="J169">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K169">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="L169">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M169">
         <v>2</v>
       </c>
       <c r="N169">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O169">
         <v>0.1</v>
@@ -22918,22 +22916,22 @@
         <v>0.967741935483871</v>
       </c>
       <c r="I171" s="3">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="J171" s="3">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="K171" s="3">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="L171" s="3">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="M171" s="3">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N171" s="3">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O171" s="3">
         <v>0.2</v>
@@ -22971,22 +22969,22 @@
         <v>245</v>
       </c>
       <c r="H172">
-        <v>0.43846153846153801</v>
+        <v>-0.36153846153846098</v>
       </c>
       <c r="I172">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="J172">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K172">
-        <v>5.3846153846153801E-2</v>
+        <v>-0.74615384615384595</v>
       </c>
       <c r="L172">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="M172">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N172">
         <v>1.3076923076922999</v>
@@ -23033,7 +23031,7 @@
         <v>0.25</v>
       </c>
       <c r="I173" s="3">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="J173" s="3">
         <v>0.125</v>
@@ -23048,7 +23046,7 @@
         <v>0.125</v>
       </c>
       <c r="N173" s="3">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="O173" s="3">
         <v>0.7</v>
@@ -23151,7 +23149,7 @@
         <v>0.98913043478260798</v>
       </c>
       <c r="I175">
-        <v>-1.30434782608695E-2</v>
+        <v>-0.81304347826086898</v>
       </c>
       <c r="J175">
         <v>0.16847826086956499</v>
@@ -23160,13 +23158,13 @@
         <v>0.16847826086956499</v>
       </c>
       <c r="L175">
-        <v>2.4999999999999901E-2</v>
+        <v>-0.77500000000000002</v>
       </c>
       <c r="M175">
-        <v>2.4999999999999901E-2</v>
+        <v>-0.77500000000000002</v>
       </c>
       <c r="N175">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O175">
         <v>-0.69999999999999896</v>
@@ -23207,25 +23205,25 @@
         <v>249</v>
       </c>
       <c r="H176">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="I176">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="J176">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="K176">
         <v>0.83333333333333304</v>
       </c>
       <c r="L176">
-        <v>0.233333333333333</v>
+        <v>-0.56666666666666599</v>
       </c>
       <c r="M176">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="N176">
-        <v>-0.2</v>
+        <v>-1.8</v>
       </c>
       <c r="O176">
         <v>-0.65</v>

</xml_diff>